<commit_message>
last version of the report
</commit_message>
<xml_diff>
--- a/Report/PANGEAHIVsim_EvaluationSheet_November.xlsx
+++ b/Report/PANGEAHIVsim_EvaluationSheet_November.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="1340" windowWidth="38640" windowHeight="19620" tabRatio="500"/>
+    <workbookView xWindow="20240" yWindow="3800" windowWidth="38640" windowHeight="19620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -541,8 +541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -695,6 +695,9 @@
       <c r="C6" t="s">
         <v>43</v>
       </c>
+      <c r="D6">
+        <v>200</v>
+      </c>
       <c r="E6">
         <v>1</v>
       </c>
@@ -709,6 +712,9 @@
       <c r="C7" t="s">
         <v>43</v>
       </c>
+      <c r="D7">
+        <v>100</v>
+      </c>
       <c r="E7">
         <v>1</v>
       </c>
@@ -723,8 +729,11 @@
       <c r="C8" t="s">
         <v>43</v>
       </c>
+      <c r="D8">
+        <v>100</v>
+      </c>
       <c r="E8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -737,6 +746,12 @@
       <c r="C9" t="s">
         <v>43</v>
       </c>
+      <c r="D9">
+        <v>200</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:17">
       <c r="A10" t="s">
@@ -748,6 +763,12 @@
       <c r="C10" t="s">
         <v>43</v>
       </c>
+      <c r="D10">
+        <v>300</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:17">
       <c r="A11" t="s">
@@ -758,6 +779,12 @@
       </c>
       <c r="C11" t="s">
         <v>43</v>
+      </c>
+      <c r="D11">
+        <v>200</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>